<commit_message>
Add the new PhysicalServerModelName property
</commit_message>
<xml_diff>
--- a/resources/templates/template_cluster.xlsx
+++ b/resources/templates/template_cluster.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">Physical Hosts</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t xml:space="preserve">VirtualizationNode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PhysicalServerModelName</t>
   </si>
   <si>
     <t xml:space="preserve">CappedCPU</t>
@@ -141,19 +144,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.05"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -169,11 +172,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>